<commit_message>
test upload for #1
Test upload build 9.
</commit_message>
<xml_diff>
--- a/Test/Build 9/TAS eBill Defect Log IB_2.0_623.xlsx
+++ b/Test/Build 9/TAS eBill Defect Log IB_2.0_623.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\eBilling Docs\Build 7&amp;8&amp;9\Docs\All\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaisathompv\Documents\github docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA0D453-CF04-4CAB-A0AD-97CDD2E849AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158BA7D3-3364-4914-AFC8-D25A0A9776C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="1875" windowWidth="20100" windowHeight="9645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="144">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>DE1499</t>
+  </si>
+  <si>
+    <t>Sandboxtest</t>
   </si>
 </sst>
 </file>
@@ -2040,14 +2043,14 @@
       <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="21.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>0</v>
       </c>
@@ -2059,10 +2062,10 @@
       <c r="G5" s="45"/>
       <c r="H5" s="45"/>
     </row>
-    <row r="6" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>27</v>
       </c>
@@ -2074,49 +2077,49 @@
       <c r="G7" s="47"/>
       <c r="H7" s="47"/>
     </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>127</v>
       </c>
@@ -2128,15 +2131,15 @@
       <c r="G23" s="48"/>
       <c r="H23" s="48"/>
     </row>
-    <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="49" t="s">
         <v>128</v>
       </c>
@@ -2148,22 +2151,22 @@
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
     </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
     </row>
   </sheetData>
@@ -2187,16 +2190,16 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="7" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
@@ -2204,7 +2207,7 @@
       <c r="C2" s="50"/>
       <c r="D2" s="50"/>
     </row>
-    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>117</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>127</v>
       </c>
@@ -2246,55 +2249,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="13"/>
       <c r="C6" s="16"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="13"/>
       <c r="C7" s="16"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
     </row>
-    <row r="9" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
     </row>
-    <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
     </row>
-    <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
     </row>
-    <row r="13" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
     </row>
-    <row r="14" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -2314,28 +2317,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="38" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="38" customWidth="1"/>
     <col min="3" max="3" width="37" style="37" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="37" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" style="37" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="37" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" style="37" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" style="37" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="37" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="37" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" style="37" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="37" customWidth="1"/>
     <col min="10" max="10" width="30" style="37" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="8"/>
+    <col min="11" max="16384" width="10.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
@@ -2367,45 +2370,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" s="29"/>
-    </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>8</v>
@@ -2414,28 +2401,28 @@
         <v>19</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="30"/>
-    </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="J3" s="29"/>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>8</v>
@@ -2444,30 +2431,28 @@
         <v>19</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>33</v>
+        <v>76</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="44" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="J4" s="30"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>8</v>
@@ -2476,28 +2461,30 @@
         <v>19</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="43"/>
-    </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>8</v>
@@ -2506,28 +2493,28 @@
         <v>19</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="30"/>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="J6" s="43"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>8</v>
@@ -2549,15 +2536,15 @@
       </c>
       <c r="J7" s="30"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>8</v>
@@ -2566,7 +2553,7 @@
         <v>19</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>39</v>
@@ -2575,22 +2562,22 @@
         <v>40</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>19</v>
@@ -2599,57 +2586,55 @@
         <v>79</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J9" s="30"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>8</v>
@@ -2658,28 +2643,30 @@
         <v>19</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="I11" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J11" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>8</v>
@@ -2688,7 +2675,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" s="28" t="s">
         <v>39</v>
@@ -2697,28 +2684,28 @@
         <v>40</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J12" s="30"/>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>39</v>
@@ -2731,15 +2718,15 @@
       </c>
       <c r="J13" s="30"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>20</v>
@@ -2748,7 +2735,7 @@
         <v>19</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>39</v>
@@ -2757,22 +2744,22 @@
         <v>40</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>19</v>
@@ -2781,64 +2768,64 @@
         <v>84</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E17" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>39</v>
@@ -2847,22 +2834,22 @@
         <v>40</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E18" s="28" t="s">
         <v>19</v>
@@ -2877,22 +2864,22 @@
         <v>40</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E19" s="28" t="s">
         <v>19</v>
@@ -2911,114 +2898,114 @@
       </c>
       <c r="J19" s="30"/>
     </row>
-    <row r="20" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E20" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="28" t="s">
         <v>97</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>20</v>
+        <v>100</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>8</v>
+        <v>104</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>20</v>
       </c>
       <c r="E23" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G23" s="28" t="s">
         <v>106</v>
@@ -3031,24 +3018,24 @@
       </c>
       <c r="J23" s="30"/>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>21</v>
+        <v>109</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>106</v>
@@ -3057,28 +3044,28 @@
         <v>107</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>8</v>
+        <v>119</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>106</v>
@@ -3087,19 +3074,19 @@
         <v>107</v>
       </c>
       <c r="I25" s="28" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="J25" s="30"/>
     </row>
-    <row r="26" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D26" s="42" t="s">
         <v>8</v>
@@ -3117,20 +3104,19 @@
         <v>107</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="J26" s="39"/>
-      <c r="M26" s="41"/>
-    </row>
-    <row r="27" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D27" s="42" t="s">
         <v>8</v>
@@ -3139,7 +3125,7 @@
         <v>19</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G27" s="28" t="s">
         <v>106</v>
@@ -3148,19 +3134,20 @@
         <v>107</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="J27" s="30"/>
-    </row>
-    <row r="28" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="J27" s="39"/>
+      <c r="M27" s="41"/>
+    </row>
+    <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D28" s="42" t="s">
         <v>8</v>
@@ -3169,7 +3156,7 @@
         <v>19</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G28" s="28" t="s">
         <v>106</v>
@@ -3182,15 +3169,15 @@
       </c>
       <c r="J28" s="30"/>
     </row>
-    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>8</v>
@@ -3212,15 +3199,15 @@
       </c>
       <c r="J29" s="30"/>
     </row>
-    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" s="42" t="s">
         <v>8</v>
@@ -3242,15 +3229,15 @@
       </c>
       <c r="J30" s="30"/>
     </row>
-    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>8</v>
@@ -3272,19 +3259,37 @@
       </c>
       <c r="J31" s="30"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="28"/>
+    <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.2">
+      <c r="A32" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J32" s="30"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -3292,50 +3297,50 @@
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
-      <c r="H33" s="36"/>
+      <c r="H33" s="35"/>
       <c r="I33" s="28"/>
       <c r="J33" s="30"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="27"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
-      <c r="H34" s="40"/>
+      <c r="H34" s="36"/>
       <c r="I34" s="28"/>
       <c r="J34" s="30"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="33"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="33"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="32"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
-      <c r="H35" s="31"/>
+      <c r="H35" s="40"/>
       <c r="I35" s="28"/>
       <c r="J35" s="30"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="33"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="36"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="30"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="28"/>
       <c r="J36" s="30"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="33"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
@@ -3344,10 +3349,10 @@
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="33"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="33"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
@@ -3356,19 +3361,19 @@
       <c r="I38" s="30"/>
       <c r="J38" s="30"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="33"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="28"/>
       <c r="E39" s="28"/>
-      <c r="F39" s="33"/>
+      <c r="F39" s="28"/>
       <c r="G39" s="28"/>
-      <c r="H39" s="33"/>
+      <c r="H39" s="36"/>
       <c r="I39" s="30"/>
       <c r="J39" s="30"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="27"/>
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
@@ -3376,23 +3381,23 @@
       <c r="E40" s="28"/>
       <c r="F40" s="33"/>
       <c r="G40" s="28"/>
-      <c r="H40" s="36"/>
+      <c r="H40" s="33"/>
       <c r="I40" s="30"/>
       <c r="J40" s="30"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="33"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="33"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="27"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
       <c r="F41" s="33"/>
       <c r="G41" s="28"/>
-      <c r="H41" s="33"/>
+      <c r="H41" s="36"/>
       <c r="I41" s="30"/>
       <c r="J41" s="30"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="33"/>
       <c r="B42" s="34"/>
       <c r="C42" s="33"/>
@@ -3404,7 +3409,7 @@
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="33"/>
       <c r="B43" s="34"/>
       <c r="C43" s="33"/>
@@ -3412,11 +3417,11 @@
       <c r="E43" s="28"/>
       <c r="F43" s="33"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="36"/>
+      <c r="H43" s="33"/>
       <c r="I43" s="30"/>
       <c r="J43" s="30"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="33"/>
       <c r="B44" s="34"/>
       <c r="C44" s="33"/>
@@ -3424,23 +3429,23 @@
       <c r="E44" s="28"/>
       <c r="F44" s="33"/>
       <c r="G44" s="28"/>
-      <c r="H44" s="34"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="30"/>
       <c r="J44" s="30"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="33"/>
       <c r="D45" s="28"/>
       <c r="E45" s="28"/>
       <c r="F45" s="33"/>
       <c r="G45" s="28"/>
-      <c r="H45" s="33"/>
+      <c r="H45" s="34"/>
       <c r="I45" s="30"/>
       <c r="J45" s="30"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="33"/>
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
@@ -3452,7 +3457,7 @@
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
@@ -3460,11 +3465,11 @@
       <c r="E47" s="28"/>
       <c r="F47" s="33"/>
       <c r="G47" s="28"/>
-      <c r="H47" s="34"/>
+      <c r="H47" s="33"/>
       <c r="I47" s="30"/>
       <c r="J47" s="30"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
@@ -3472,11 +3477,11 @@
       <c r="E48" s="28"/>
       <c r="F48" s="33"/>
       <c r="G48" s="28"/>
-      <c r="H48" s="40"/>
+      <c r="H48" s="34"/>
       <c r="I48" s="30"/>
       <c r="J48" s="30"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="33"/>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
@@ -3488,7 +3493,7 @@
       <c r="I49" s="30"/>
       <c r="J49" s="30"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="33"/>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
@@ -3500,7 +3505,7 @@
       <c r="I50" s="30"/>
       <c r="J50" s="30"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="33"/>
       <c r="B51" s="33"/>
       <c r="C51" s="33"/>
@@ -3512,7 +3517,7 @@
       <c r="I51" s="30"/>
       <c r="J51" s="30"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="33"/>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
@@ -3524,10 +3529,10 @@
       <c r="I52" s="30"/>
       <c r="J52" s="30"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="33"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
       <c r="D53" s="28"/>
       <c r="E53" s="28"/>
       <c r="F53" s="33"/>
@@ -3536,7 +3541,7 @@
       <c r="I53" s="30"/>
       <c r="J53" s="30"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
@@ -3544,23 +3549,23 @@
       <c r="E54" s="28"/>
       <c r="F54" s="33"/>
       <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="33"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="30"/>
       <c r="J54" s="30"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="30"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="33"/>
       <c r="J55" s="30"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -3572,15 +3577,27 @@
       <c r="I56" s="30"/>
       <c r="J56" s="30"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="37"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="30"/>
+      <c r="J57" s="30"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="37"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H29">
-    <sortCondition descending="1" ref="A2:A29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H30">
+    <sortCondition descending="1" ref="A3:A30"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="/79590444732d/detail/defect/148456306180" display="/79590444732d/detail/defect/148456306180" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId1" location="/79590444732d/detail/defect/148456306180" display="/79590444732d/detail/defect/148456306180" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>